<commit_message>
V3 of the lean canvas
Update to canvas and scoring before the silly season, happy holidays all!
</commit_message>
<xml_diff>
--- a/data_ventures_lean_canvas.xlsx
+++ b/data_ventures_lean_canvas.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>DV lean canvas: Data Ventures</t>
   </si>
@@ -31,17 +31,17 @@
     <t>Customer segments</t>
   </si>
   <si>
-    <t>Data drived so many policy decisions and solutions. Getting access to data can be tricky. This means that there are gaps in the data.
+    <t>Data drives so many policy decisions and solutions. Getting access to data can be tricky. This means that there are gaps in the data, especially data used to measure performance of investments over time.
 Currently, the only option is to get one-off access from one source. This is expensive and time consuming for everyone.
 There are very few trusted, neutral and impartial parties that can bring open government and private data together.
-When providing data to government, there is a risk that the government agency receiving the data can react with legaslative and regulatory changes impacting the data providers heavily.</t>
+When providing data to government, there is a risk that the government agency receiving the data can react with legislative and regulatory changes impacting the data providers heavily.</t>
   </si>
   <si>
     <t>A commercially focused Stats NZ business unit allows us to: 
 * give value back to the data suppliers, 
 * bring competing data sets together for the first time, 
 * be trusted to look after the privacy of the data sets, protecting all parties involved.
-Data suppliers will provide us with data. We will standardise, confidentialise, and provide assurances to it and then make it accessible according to the various maturity levels of the customers (it could be a data stream, or it could be a basic web application). Customers can provide feedback to help us improve.
+Data suppliers will provide us with aggregated data based on the use case. We will standardise, confidentialised, and provide assurances to it and then make it accessible according to the various maturity levels of the customers (it could be a data stream, or it could be a basic web application). Customers can provide feedback to help us improve.
 We will bring together open government data and private commercial data to create new and improved value.</t>
   </si>
   <si>
@@ -65,7 +65,8 @@
 Crown Entities
 Iwi
 Council-controlled organisations
-Council-controlled trading organisations</t>
+Council-controlled trading organisations
+Other customer groups discovered through the pilot</t>
   </si>
   <si>
     <t>Existing alternatives</t>
@@ -115,7 +116,7 @@
     <t xml:space="preserve">The core costs of running of Data Ventures will come from the core team and some business as usual (BAU) costs (such as software subscriptions, stationary, toilet paper, etc.) and hiring a team.
 We have levers in the business model which attributes to the running costs of the data brokerage model:
 * Short term return to data providers, a fixed amount (either annual or one off) that we provide to offset their initial investment on the work required to shape/process the data sets we require, i.e. to create certain anonymising and classifications based on the data
-* Long term return to data providers, a % share of revenue of the use case.
+* Long term return to data providers, a % share of revenue of the use case, access to the aggregated dataset, leverage of DV market research as a value add channel
 Marketing and PR are essential to managing perceptions and ensuring stakeholders are appropriately kept up to date. If we get this wrong,  people assume we are doing bad things (which we aren't) e.g. selling Stats NZ data.
 Technology costs (marketing / hosting / tools and apps).              </t>
   </si>
@@ -124,6 +125,15 @@
 Two revenue streams, monthly subscriptions from products and services based on the data brokerage model. One-off on demand customers are for specific use cases, such as Civil Defense in an emergency. This is not a standard or open offering.
 Environment/Economic returns: Unlocking data sets normally unobtainable to allow more beneficial decisions impacting Aotearoa New Zealand.
 Social returns: 1+1 Model; allow smaller customers to be able to afford access to the data sets, such as pricing higher for customers with larger allocations of budget/cash to then offset. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scoring
+Effort: 6 - Enterprise sales in a condensed period of time and the funding cycle associated with government. Limitation in our complexity due to limiting our sales channel to govt only
+Acquisition:  6 - We have developed an operating model that considers what's in it for the data providers, DV and the public benefits. It's a case of using this now to develop any further relationships for new and existing data providers for future products. We will have to do some acquisition of either internal resources or contractors or seconded but either way it's not that hard
+Risk: 6 - We have mitigation plans of things we have control of. The risk associated is through lack of control over third parties.
+Complexity: 6 - Unknown complexities around long term commercial arrangements between DV and customers and DV and data providers.
+Value: 8 - DV views the value to bit high, but customers and data providers need help to understand that value.
 </t>
   </si>
 </sst>
@@ -305,9 +315,15 @@
         <v>20</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A7:E7"/>
   </mergeCells>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>